<commit_message>
pom.xml changes and screenshot changes
</commit_message>
<xml_diff>
--- a/CucumberBaseFramework/src/test/resources/TestData/TestCase.xlsx
+++ b/CucumberBaseFramework/src/test/resources/TestData/TestCase.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TheGeneral\GitHub\cucumber_Selenium_java\CucumberBaseFramework\src\test\resources\TestData\"/>
     </mc:Choice>
@@ -16,7 +16,7 @@
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="45">
   <si>
     <t>Type</t>
   </si>
@@ -75,13 +75,98 @@
   </si>
   <si>
     <t xml:space="preserve">Policy Type </t>
+  </si>
+  <si>
+    <t>TN2485352</t>
+  </si>
+  <si>
+    <t>11539914</t>
+  </si>
+  <si>
+    <t>Base</t>
+  </si>
+  <si>
+    <t>TC002</t>
+  </si>
+  <si>
+    <t>TN2485356</t>
+  </si>
+  <si>
+    <t>11539933</t>
+  </si>
+  <si>
+    <t>TB2485358</t>
+  </si>
+  <si>
+    <t>11539965</t>
+  </si>
+  <si>
+    <t>Nil</t>
+  </si>
+  <si>
+    <t>TC001</t>
+  </si>
+  <si>
+    <t>TN2485359</t>
+  </si>
+  <si>
+    <t>11539970</t>
+  </si>
+  <si>
+    <t>TN2485361</t>
+  </si>
+  <si>
+    <t>11539983</t>
+  </si>
+  <si>
+    <t>TN2485363</t>
+  </si>
+  <si>
+    <t>11540001</t>
+  </si>
+  <si>
+    <t>TN2485392</t>
+  </si>
+  <si>
+    <t>11540661</t>
+  </si>
+  <si>
+    <t>TN2485397</t>
+  </si>
+  <si>
+    <t>11540740</t>
+  </si>
+  <si>
+    <t>TN2485399</t>
+  </si>
+  <si>
+    <t>11540748</t>
+  </si>
+  <si>
+    <t>TN2485403</t>
+  </si>
+  <si>
+    <t>11540787</t>
+  </si>
+  <si>
+    <t>TN2485405</t>
+  </si>
+  <si>
+    <t>11540797</t>
+  </si>
+  <si>
+    <t>TN2485407</t>
+  </si>
+  <si>
+    <t>11540814</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -400,11 +485,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.140625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="15" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="22.140625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="15.42578125" customWidth="1"/>
-    <col min="5" max="5" width="15.42578125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="16.140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="15.0" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="22.140625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="15.42578125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="15.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -468,6 +553,210 @@
         <v>3</v>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" t="s">
+        <v>1</v>
+      </c>
+      <c r="D8" t="s">
+        <v>25</v>
+      </c>
+      <c r="E8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" t="s">
+        <v>2</v>
+      </c>
+      <c r="D9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D10" t="s">
+        <v>5</v>
+      </c>
+      <c r="E10" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" t="s">
+        <v>2</v>
+      </c>
+      <c r="D11" t="s">
+        <v>5</v>
+      </c>
+      <c r="E11" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" t="s">
+        <v>2</v>
+      </c>
+      <c r="D12" t="s">
+        <v>5</v>
+      </c>
+      <c r="E12" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>35</v>
+      </c>
+      <c r="B13" t="s">
+        <v>36</v>
+      </c>
+      <c r="C13" t="s">
+        <v>2</v>
+      </c>
+      <c r="D13" t="s">
+        <v>19</v>
+      </c>
+      <c r="E13" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>37</v>
+      </c>
+      <c r="B14" t="s">
+        <v>38</v>
+      </c>
+      <c r="C14" t="s">
+        <v>2</v>
+      </c>
+      <c r="D14" t="s">
+        <v>19</v>
+      </c>
+      <c r="E14" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>39</v>
+      </c>
+      <c r="B15" t="s">
+        <v>40</v>
+      </c>
+      <c r="C15" t="s">
+        <v>2</v>
+      </c>
+      <c r="D15" t="s">
+        <v>19</v>
+      </c>
+      <c r="E15" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>41</v>
+      </c>
+      <c r="B16" t="s">
+        <v>42</v>
+      </c>
+      <c r="C16" t="s">
+        <v>2</v>
+      </c>
+      <c r="D16" t="s">
+        <v>19</v>
+      </c>
+      <c r="E16" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s">
+        <v>43</v>
+      </c>
+      <c r="B17" t="s">
+        <v>44</v>
+      </c>
+      <c r="C17" t="s">
+        <v>2</v>
+      </c>
+      <c r="D17" t="s">
+        <v>19</v>
+      </c>
+      <c r="E17" t="s">
+        <v>20</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
changes made in base class and config.proprty
</commit_message>
<xml_diff>
--- a/CucumberBaseFramework/src/test/resources/TestData/TestCase.xlsx
+++ b/CucumberBaseFramework/src/test/resources/TestData/TestCase.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="63">
   <si>
     <t>Type</t>
   </si>
@@ -201,6 +201,18 @@
   </si>
   <si>
     <t>11541995</t>
+  </si>
+  <si>
+    <t>TB2485446</t>
+  </si>
+  <si>
+    <t>11542176</t>
+  </si>
+  <si>
+    <t>TN2485447</t>
+  </si>
+  <si>
+    <t>11542189</t>
   </si>
 </sst>
 </file>
@@ -901,6 +913,40 @@
         <v>20</v>
       </c>
     </row>
+    <row r="24">
+      <c r="A24" t="s">
+        <v>59</v>
+      </c>
+      <c r="B24" t="s">
+        <v>60</v>
+      </c>
+      <c r="C24" t="s">
+        <v>1</v>
+      </c>
+      <c r="D24" t="s">
+        <v>25</v>
+      </c>
+      <c r="E24" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="s">
+        <v>61</v>
+      </c>
+      <c r="B25" t="s">
+        <v>62</v>
+      </c>
+      <c r="C25" t="s">
+        <v>2</v>
+      </c>
+      <c r="D25" t="s">
+        <v>19</v>
+      </c>
+      <c r="E25" t="s">
+        <v>20</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>